<commit_message>
Update statistic page + reload data
</commit_message>
<xml_diff>
--- a/excel/ThongKeDoanhThu_2023.xlsx
+++ b/excel/ThongKeDoanhThu_2023.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Doanh thu năm 2023" r:id="rId3" sheetId="1"/>
+    <sheet name="Doanh thu 2023" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Tháng</t>
   </si>
@@ -41,7 +41,13 @@
     <t>Tháng 7</t>
   </si>
   <si>
+    <t>Tháng 8</t>
+  </si>
+  <si>
     <t>Tháng 9</t>
+  </si>
+  <si>
+    <t>Tháng 10</t>
   </si>
   <si>
     <t>Tháng 11</t>
@@ -101,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -120,91 +126,107 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="n" s="0">
-        <v>190000.0</v>
+      <c r="B2" t="n">
+        <v>245000.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="n" s="0">
-        <v>120000.0</v>
+      <c r="B3" t="n">
+        <v>300000.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n" s="0">
-        <v>185000.0</v>
+      <c r="B4" t="n">
+        <v>395000.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="n" s="0">
-        <v>220000.0</v>
+      <c r="B5" t="n">
+        <v>390000.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="n" s="0">
-        <v>265000.0</v>
+      <c r="B6" t="n">
+        <v>455000.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n" s="0">
-        <v>145000.0</v>
+      <c r="B7" t="n">
+        <v>345000.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="n" s="0">
-        <v>200000.0</v>
+      <c r="B8" t="n">
+        <v>430000.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="n" s="0">
-        <v>300000.0</v>
+      <c r="B9" t="n">
+        <v>260000.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="n" s="0">
-        <v>90000.0</v>
+      <c r="B10" t="n">
+        <v>485000.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="n" s="0">
-        <v>180000.0</v>
+      <c r="B11" t="n">
+        <v>175000.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>245000.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n" s="0">
-        <v>1895000.0</v>
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>400000.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4125000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>